<commit_message>
changed index values with variable names
</commit_message>
<xml_diff>
--- a/excel_parser/generate-files.xlsx
+++ b/excel_parser/generate-files.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="01-epics" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="02-stories" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="epic_stories" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="epic_stories1" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="gen_sheet" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -18,9 +18,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -51,11 +50,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,7 +580,7 @@
   </sheetPr>
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
@@ -1378,1458 +1376,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:Y15"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="23.140625" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="21.42578125" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="21.5703125" bestFit="1" customWidth="1" min="8" max="8"/>
-    <col width="26" bestFit="1" customWidth="1" min="9" max="9"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>s.no</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>STORY ID</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Issue id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>EPIC ID</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>ESdate</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>STORY
-PLANNED
-START</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>STORY
-PLANNED
-END</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>STORY
-ACTUAL
-START</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>STORY
-ACTUAL
-END</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>ASSIGNED TO</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>STORY
-Effort
-completion
-%</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>ESTIMATED
-STORY
-POINTS</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Time spent
-(IN Secs)</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>EFFORT
-CONSUMED
-(IN HRS)</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>Time Spent</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>ESTIMATED
-EFFORT
-(IN HRS))</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>Remaining Estimate</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>PENDING
-EFFORT
-(IN HRS)</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>SPRINT ID</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>Sprint2</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>Sprint3</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">STORY
-Schedule
-Progress % </t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>STORY
-Schedule
-Overrun %</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>Remarks</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>STORY DESCRIPTION</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>PCS-27974</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>594882</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>PCS-28018</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>May21-Performance</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>balachandras</t>
-        </is>
-      </c>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" t="n">
-        <v>57600</v>
-      </c>
-      <c r="N2" t="n">
-        <v>16</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>57600</v>
-      </c>
-      <c r="R2" t="n">
-        <v>16</v>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>QA: Testing the throughput with standard/less packet sizes/varied user load in ESP mode</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>PCS-27972</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>594870</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>PCS-28018</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>May21-Performance</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>balachandras</t>
-        </is>
-      </c>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" t="n">
-        <v>4</v>
-      </c>
-      <c r="M3" t="n">
-        <v>57600</v>
-      </c>
-      <c r="N3" t="n">
-        <v>16</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>57600</v>
-      </c>
-      <c r="R3" t="n">
-        <v>16</v>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">QA:SM HW : ESP Max Users/Tunnel Setup count </t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>PCS-27539</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>593251</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>PCS-28018</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>May21-Performance</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>balachandras</t>
-        </is>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>4</v>
-      </c>
-      <c r="M4" t="n">
-        <v>57600</v>
-      </c>
-      <c r="N4" t="n">
-        <v>16</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>57600</v>
-      </c>
-      <c r="R4" t="n">
-        <v>16</v>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>Planning to validate RAID and LVM testing</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>PCS-25735</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>583642</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>PCS-28018</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>May21-Performance</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>balachandras</t>
-        </is>
-      </c>
-      <c r="K5" t="n">
-        <v>75</v>
-      </c>
-      <c r="L5" t="n">
-        <v>4</v>
-      </c>
-      <c r="M5" t="n">
-        <v>57600</v>
-      </c>
-      <c r="N5" t="n">
-        <v>16</v>
-      </c>
-      <c r="O5" t="n">
-        <v>43200</v>
-      </c>
-      <c r="P5" t="n">
-        <v>12</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>57600</v>
-      </c>
-      <c r="R5" t="n">
-        <v>16</v>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>PCS-2112</t>
-        </is>
-      </c>
-      <c r="V5" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>QA: Testing the HW-RAID controller functionality</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>PCS-28004</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>594947</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>PCS-28042</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>44261</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H6" s="2" t="n">
-        <v>44261</v>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>May21-ISA8000x-Support</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>balajit</t>
-        </is>
-      </c>
-      <c r="K6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" t="n">
-        <v>4</v>
-      </c>
-      <c r="M6" t="n">
-        <v>57600</v>
-      </c>
-      <c r="N6" t="n">
-        <v>16</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>57600</v>
-      </c>
-      <c r="R6" t="n">
-        <v>16</v>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>SM HW - ISA8000F Platform Testing, Code Review</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>PCS-28003</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>594946</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>PCS-28042</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F7" s="2" t="n">
-        <v>44261</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H7" s="2" t="n">
-        <v>44261</v>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>May21-ISA8000x-Support</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>balajit</t>
-        </is>
-      </c>
-      <c r="K7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" t="n">
-        <v>4</v>
-      </c>
-      <c r="M7" t="n">
-        <v>57600</v>
-      </c>
-      <c r="N7" t="n">
-        <v>16</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P7" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>57600</v>
-      </c>
-      <c r="R7" t="n">
-        <v>16</v>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y7" t="inlineStr">
-        <is>
-          <t>SM HW - ISA8000F Platform addition - License and UI Changes</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>PCS-28002</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>594945</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>PCS-28042</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F8" s="2" t="n">
-        <v>44261</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H8" s="2" t="n">
-        <v>44261</v>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>May21-ISA8000x-Support</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>balajit</t>
-        </is>
-      </c>
-      <c r="K8" t="n">
-        <v>96</v>
-      </c>
-      <c r="L8" t="n">
-        <v>6</v>
-      </c>
-      <c r="M8" t="n">
-        <v>86400</v>
-      </c>
-      <c r="N8" t="n">
-        <v>24</v>
-      </c>
-      <c r="O8" t="n">
-        <v>82800</v>
-      </c>
-      <c r="P8" t="n">
-        <v>23</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>3600</v>
-      </c>
-      <c r="R8" t="n">
-        <v>1</v>
-      </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="V8" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W8" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y8" t="inlineStr">
-        <is>
-          <t>SM HW - ISA8000F Platform addition - Platform changes</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>PCS-27971</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>594869</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>PCS-28017</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F9" s="2" t="n">
-        <v>44261</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H9" s="2" t="n">
-        <v>44261</v>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>May21-Deployment-Phase2</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>kalaimani.k</t>
-        </is>
-      </c>
-      <c r="K9" t="n">
-        <v>100</v>
-      </c>
-      <c r="L9" t="n">
-        <v>4</v>
-      </c>
-      <c r="M9" t="n">
-        <v>57600</v>
-      </c>
-      <c r="N9" t="n">
-        <v>16</v>
-      </c>
-      <c r="O9" t="n">
-        <v>57600</v>
-      </c>
-      <c r="P9" t="n">
-        <v>16</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>0</v>
-      </c>
-      <c r="R9" t="n">
-        <v>0</v>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="V9" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W9" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">SM-HW : ISA8000 - Make Coreboot/init changes as platform specific  </t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>PCS-27007</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>590473</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>PCS-28017</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F10" s="2" t="n">
-        <v>44261</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H10" s="2" t="n">
-        <v>44261</v>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>May21-Deployment-Phase2</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>kalaimani.k</t>
-        </is>
-      </c>
-      <c r="K10" t="n">
-        <v>25</v>
-      </c>
-      <c r="L10" t="n">
-        <v>8</v>
-      </c>
-      <c r="M10" t="n">
-        <v>115200</v>
-      </c>
-      <c r="N10" t="n">
-        <v>32</v>
-      </c>
-      <c r="O10" t="n">
-        <v>28800</v>
-      </c>
-      <c r="P10" t="n">
-        <v>8</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>86400</v>
-      </c>
-      <c r="R10" t="n">
-        <v>24</v>
-      </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>PCS-2118</t>
-        </is>
-      </c>
-      <c r="T10" t="inlineStr">
-        <is>
-          <t>PCS-2120</t>
-        </is>
-      </c>
-      <c r="U10" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="V10" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W10" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">SM-HW: ISA8000 Upgrade and Rollover Confirmation with LVM </t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>PCS-27969</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>594853</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>PCS-28017</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F11" s="2" t="n">
-        <v>44261</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H11" s="2" t="n">
-        <v>44261</v>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>May21-Deployment-Phase2</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>kalaimani.k</t>
-        </is>
-      </c>
-      <c r="K11" t="n">
-        <v>0</v>
-      </c>
-      <c r="L11" t="n">
-        <v>4</v>
-      </c>
-      <c r="M11" t="n">
-        <v>57600</v>
-      </c>
-      <c r="N11" t="n">
-        <v>16</v>
-      </c>
-      <c r="O11" t="n">
-        <v>0</v>
-      </c>
-      <c r="P11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>57600</v>
-      </c>
-      <c r="R11" t="n">
-        <v>16</v>
-      </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="V11" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W11" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y11" t="inlineStr">
-        <is>
-          <t>LVM: Support and bug fixes</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>PCS-27566</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>593427</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>PCS-28018</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>May21-Performance</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>karthikr</t>
-        </is>
-      </c>
-      <c r="K12" t="n">
-        <v>0</v>
-      </c>
-      <c r="L12" t="n">
-        <v>4</v>
-      </c>
-      <c r="M12" t="n">
-        <v>28800</v>
-      </c>
-      <c r="N12" t="n">
-        <v>8</v>
-      </c>
-      <c r="O12" t="n">
-        <v>0</v>
-      </c>
-      <c r="P12" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>28800</v>
-      </c>
-      <c r="R12" t="n">
-        <v>8</v>
-      </c>
-      <c r="S12" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="V12" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W12" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">QA: SMHW: Tunnel setup rate test for 25k Users on SSL mode </t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>PCS-27538</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>593250</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>PCS-28018</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>May21-Performance</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>karthikr</t>
-        </is>
-      </c>
-      <c r="K13" t="n">
-        <v>0</v>
-      </c>
-      <c r="L13" t="n">
-        <v>4</v>
-      </c>
-      <c r="M13" t="n">
-        <v>57600</v>
-      </c>
-      <c r="N13" t="n">
-        <v>16</v>
-      </c>
-      <c r="O13" t="n">
-        <v>0</v>
-      </c>
-      <c r="P13" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>57600</v>
-      </c>
-      <c r="R13" t="n">
-        <v>16</v>
-      </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="V13" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W13" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y13" t="inlineStr">
-        <is>
-          <t>QA: SM HW : Perform throughput tests with IMIX traffic(SSL)</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>PCS-27978</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>594893</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>PCS-28018</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>May21-Performance</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>karthikr</t>
-        </is>
-      </c>
-      <c r="K14" t="n">
-        <v>0</v>
-      </c>
-      <c r="L14" t="n">
-        <v>4</v>
-      </c>
-      <c r="M14" t="n">
-        <v>57600</v>
-      </c>
-      <c r="N14" t="n">
-        <v>16</v>
-      </c>
-      <c r="O14" t="n">
-        <v>0</v>
-      </c>
-      <c r="P14" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>57600</v>
-      </c>
-      <c r="R14" t="n">
-        <v>16</v>
-      </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="V14" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W14" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y14" t="inlineStr">
-        <is>
-          <t>QA: SM HW : SSL Max Throughput (25k Users/Tunnels, 1350 bytes)</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>PCS-27975</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>594885</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>PCS-28018</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>May21-Performance</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>karthikr</t>
-        </is>
-      </c>
-      <c r="K15" t="n">
-        <v>50</v>
-      </c>
-      <c r="L15" t="n">
-        <v>2</v>
-      </c>
-      <c r="M15" t="n">
-        <v>28800</v>
-      </c>
-      <c r="N15" t="n">
-        <v>8</v>
-      </c>
-      <c r="O15" t="n">
-        <v>14400</v>
-      </c>
-      <c r="P15" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>14400</v>
-      </c>
-      <c r="R15" t="n">
-        <v>4</v>
-      </c>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="V15" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W15" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y15" t="inlineStr">
-        <is>
-          <t>QA: Build image from Build plan</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2866,35 +1412,35 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>ESdate</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
           <t>STORY
 PLANNED
 START</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>STORY
 PLANNED
 END</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>STORY
 ACTUAL
 START</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>STORY
 ACTUAL
 END</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Ename</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
@@ -3386,7 +1932,7 @@
           <t>20-05-2021</t>
         </is>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" s="2" t="n">
         <v>44261</v>
       </c>
       <c r="G6" t="inlineStr">
@@ -3394,7 +1940,7 @@
           <t>20-05-2021</t>
         </is>
       </c>
-      <c r="H6" s="3" t="n">
+      <c r="H6" s="2" t="n">
         <v>44261</v>
       </c>
       <c r="I6" t="inlineStr">
@@ -3474,7 +2020,7 @@
           <t>20-05-2021</t>
         </is>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="F7" s="2" t="n">
         <v>44261</v>
       </c>
       <c r="G7" t="inlineStr">
@@ -3482,7 +2028,7 @@
           <t>20-05-2021</t>
         </is>
       </c>
-      <c r="H7" s="3" t="n">
+      <c r="H7" s="2" t="n">
         <v>44261</v>
       </c>
       <c r="I7" t="inlineStr">
@@ -3562,7 +2108,7 @@
           <t>20-05-2021</t>
         </is>
       </c>
-      <c r="F8" s="3" t="n">
+      <c r="F8" s="2" t="n">
         <v>44261</v>
       </c>
       <c r="G8" t="inlineStr">
@@ -3570,7 +2116,7 @@
           <t>20-05-2021</t>
         </is>
       </c>
-      <c r="H8" s="3" t="n">
+      <c r="H8" s="2" t="n">
         <v>44261</v>
       </c>
       <c r="I8" t="inlineStr">
@@ -3650,7 +2196,7 @@
           <t>20-05-2021</t>
         </is>
       </c>
-      <c r="F9" s="3" t="n">
+      <c r="F9" s="2" t="n">
         <v>44261</v>
       </c>
       <c r="G9" t="inlineStr">
@@ -3658,7 +2204,7 @@
           <t>20-05-2021</t>
         </is>
       </c>
-      <c r="H9" s="3" t="n">
+      <c r="H9" s="2" t="n">
         <v>44261</v>
       </c>
       <c r="I9" t="inlineStr">
@@ -3738,7 +2284,7 @@
           <t>20-05-2021</t>
         </is>
       </c>
-      <c r="F10" s="3" t="n">
+      <c r="F10" s="2" t="n">
         <v>44261</v>
       </c>
       <c r="G10" t="inlineStr">
@@ -3746,7 +2292,7 @@
           <t>20-05-2021</t>
         </is>
       </c>
-      <c r="H10" s="3" t="n">
+      <c r="H10" s="2" t="n">
         <v>44261</v>
       </c>
       <c r="I10" t="inlineStr">
@@ -3836,7 +2382,7 @@
           <t>20-05-2021</t>
         </is>
       </c>
-      <c r="F11" s="3" t="n">
+      <c r="F11" s="2" t="n">
         <v>44261</v>
       </c>
       <c r="G11" t="inlineStr">
@@ -3844,7 +2390,7 @@
           <t>20-05-2021</t>
         </is>
       </c>
-      <c r="H11" s="3" t="n">
+      <c r="H11" s="2" t="n">
         <v>44261</v>
       </c>
       <c r="I11" t="inlineStr">
@@ -4267,6 +2813,1211 @@
       <c r="Y15" t="inlineStr">
         <is>
           <t>QA: Build image from Build plan</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:T15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>s.no</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>EPIC ID</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>SPRINT ID</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>STORY ID</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>STORY DESCRIPTION</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>ASSIGNED TO</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>ESTIMATED
+STORY
+POINTS</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>STORY
+PLANNED
+START</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>STORY
+PLANNED
+END</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>EFFORT
+CONSUMED
+(IN HRS)</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Time spent
+(IN Secs)</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>EFFORT
+CONSUMED
+(IN HRS)</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>PENDING
+EFFORT
+(IN HRS)</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>STORY
+ACTUAL
+START</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>STORY
+ACTUAL
+END</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>STORY
+Effort
+completion
+%</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">STORY
+Schedule
+Progress % </t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>STORY
+Schedule
+Overrun %</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>Remarks</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>PCS-28018</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>PCS-2122</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>PCS-27974</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>QA: Testing the throughput with standard/less packet sizes/varied user load in ESP mode</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>balachandras</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>17-06-2021</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>16</v>
+      </c>
+      <c r="K2" t="n">
+        <v>57600</v>
+      </c>
+      <c r="L2" t="n">
+        <v>16</v>
+      </c>
+      <c r="M2" t="n">
+        <v>16</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>17-06-2021</t>
+        </is>
+      </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>PCS-28018</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>PCS-2122</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>PCS-27972</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">QA:SM HW : ESP Max Users/Tunnel Setup count </t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>balachandras</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>17-06-2021</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>16</v>
+      </c>
+      <c r="K3" t="n">
+        <v>57600</v>
+      </c>
+      <c r="L3" t="n">
+        <v>16</v>
+      </c>
+      <c r="M3" t="n">
+        <v>16</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>17-06-2021</t>
+        </is>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>PCS-28018</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>PCS-2122</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>PCS-27539</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Planning to validate RAID and LVM testing</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>balachandras</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>4</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>17-06-2021</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>16</v>
+      </c>
+      <c r="K4" t="n">
+        <v>57600</v>
+      </c>
+      <c r="L4" t="n">
+        <v>16</v>
+      </c>
+      <c r="M4" t="n">
+        <v>16</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>17-06-2021</t>
+        </is>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>PCS-28018</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>PCS-2122</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>PCS-25735</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>QA: Testing the HW-RAID controller functionality</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>balachandras</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>4</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>17-06-2021</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>16</v>
+      </c>
+      <c r="K5" t="n">
+        <v>57600</v>
+      </c>
+      <c r="L5" t="n">
+        <v>16</v>
+      </c>
+      <c r="M5" t="n">
+        <v>16</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>17-06-2021</t>
+        </is>
+      </c>
+      <c r="P5" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>PCS-28042</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>PCS-2122</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>PCS-28004</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>SM HW - ISA8000F Platform Testing, Code Review</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>balajit</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>4</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>44261</v>
+      </c>
+      <c r="J6" t="n">
+        <v>16</v>
+      </c>
+      <c r="K6" t="n">
+        <v>57600</v>
+      </c>
+      <c r="L6" t="n">
+        <v>16</v>
+      </c>
+      <c r="M6" t="n">
+        <v>16</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="O6" s="2" t="n">
+        <v>44261</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>PCS-28042</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>PCS-2122</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>PCS-28003</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>SM HW - ISA8000F Platform addition - License and UI Changes</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>balajit</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>4</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>44261</v>
+      </c>
+      <c r="J7" t="n">
+        <v>16</v>
+      </c>
+      <c r="K7" t="n">
+        <v>57600</v>
+      </c>
+      <c r="L7" t="n">
+        <v>16</v>
+      </c>
+      <c r="M7" t="n">
+        <v>16</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="O7" s="2" t="n">
+        <v>44261</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>PCS-28042</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>PCS-2122</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>PCS-28002</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>SM HW - ISA8000F Platform addition - Platform changes</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>balajit</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>6</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>44261</v>
+      </c>
+      <c r="J8" t="n">
+        <v>24</v>
+      </c>
+      <c r="K8" t="n">
+        <v>86400</v>
+      </c>
+      <c r="L8" t="n">
+        <v>24</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="O8" s="2" t="n">
+        <v>44261</v>
+      </c>
+      <c r="P8" t="n">
+        <v>96</v>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>PCS-28017</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>PCS-2122</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>PCS-27971</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SM-HW : ISA8000 - Make Coreboot/init changes as platform specific  </t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>kalaimani.k</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>4</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>44261</v>
+      </c>
+      <c r="J9" t="n">
+        <v>16</v>
+      </c>
+      <c r="K9" t="n">
+        <v>57600</v>
+      </c>
+      <c r="L9" t="n">
+        <v>16</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="O9" s="2" t="n">
+        <v>44261</v>
+      </c>
+      <c r="P9" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>PCS-28017</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>PCS-2118</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>PCS-27007</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SM-HW: ISA8000 Upgrade and Rollover Confirmation with LVM </t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>kalaimani.k</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>8</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>44261</v>
+      </c>
+      <c r="J10" t="n">
+        <v>32</v>
+      </c>
+      <c r="K10" t="n">
+        <v>115200</v>
+      </c>
+      <c r="L10" t="n">
+        <v>32</v>
+      </c>
+      <c r="M10" t="n">
+        <v>24</v>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="O10" s="2" t="n">
+        <v>44261</v>
+      </c>
+      <c r="P10" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>PCS-28017</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>PCS-2122</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>PCS-27969</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LVM: Support and bug fixes</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>kalaimani.k</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>4</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>44261</v>
+      </c>
+      <c r="J11" t="n">
+        <v>16</v>
+      </c>
+      <c r="K11" t="n">
+        <v>57600</v>
+      </c>
+      <c r="L11" t="n">
+        <v>16</v>
+      </c>
+      <c r="M11" t="n">
+        <v>16</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="O11" s="2" t="n">
+        <v>44261</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>PCS-28018</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>PCS-2122</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>PCS-27566</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">QA: SMHW: Tunnel setup rate test for 25k Users on SSL mode </t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>karthikr</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>4</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>17-06-2021</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>8</v>
+      </c>
+      <c r="K12" t="n">
+        <v>28800</v>
+      </c>
+      <c r="L12" t="n">
+        <v>8</v>
+      </c>
+      <c r="M12" t="n">
+        <v>8</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>17-06-2021</t>
+        </is>
+      </c>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>PCS-28018</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>PCS-2122</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>PCS-27538</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>QA: SM HW : Perform throughput tests with IMIX traffic(SSL)</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>karthikr</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>4</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>17-06-2021</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>16</v>
+      </c>
+      <c r="K13" t="n">
+        <v>57600</v>
+      </c>
+      <c r="L13" t="n">
+        <v>16</v>
+      </c>
+      <c r="M13" t="n">
+        <v>16</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>17-06-2021</t>
+        </is>
+      </c>
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>PCS-28018</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>PCS-2122</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>PCS-27978</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>QA: SM HW : SSL Max Throughput (25k Users/Tunnels, 1350 bytes)</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>karthikr</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>4</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>17-06-2021</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>16</v>
+      </c>
+      <c r="K14" t="n">
+        <v>57600</v>
+      </c>
+      <c r="L14" t="n">
+        <v>16</v>
+      </c>
+      <c r="M14" t="n">
+        <v>16</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>17-06-2021</t>
+        </is>
+      </c>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>PCS-28018</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>PCS-2122</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>PCS-27975</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>QA: Build image from Build plan</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>karthikr</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>2</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>17-06-2021</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>8</v>
+      </c>
+      <c r="K15" t="n">
+        <v>28800</v>
+      </c>
+      <c r="L15" t="n">
+        <v>8</v>
+      </c>
+      <c r="M15" t="n">
+        <v>4</v>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>20-05-2021</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>17-06-2021</t>
+        </is>
+      </c>
+      <c r="P15" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add generate data and excel file
</commit_message>
<xml_diff>
--- a/excel_parser/generate-files.xlsx
+++ b/excel_parser/generate-files.xlsx
@@ -8,8 +8,7 @@
   <sheets>
     <sheet name="01-epics" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="02-stories" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="epic_stories" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="gen_sheet" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="stories" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -1381,1452 +1380,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>s.no</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>STORY ID</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Issue id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>EPIC ID</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>STORY
-PLANNED
-START</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>STORY
-PLANNED
-END</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>STORY
-ACTUAL
-START</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>STORY
-ACTUAL
-END</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Ename</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>ASSIGNED TO</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>STORY
-Effort
-completion
-%</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>ESTIMATED
-STORY
-POINTS</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Time spent
-(IN Secs)</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>EFFORT
-CONSUMED
-(IN HRS)</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>Time Spent</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>ESTIMATED
-EFFORT
-(IN HRS))</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>Remaining Estimate</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>PENDING
-EFFORT
-(IN HRS)</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>SPRINT ID</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>Sprint2</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>Sprint3</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">STORY
-Schedule
-Progress % </t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>STORY
-Schedule
-Overrun %</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>Remarks</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>STORY DESCRIPTION</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>PCS-27974</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>594882</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>PCS-28018</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>May21-Performance</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>balachandras</t>
-        </is>
-      </c>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" t="n">
-        <v>57600</v>
-      </c>
-      <c r="N2" t="n">
-        <v>16</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>57600</v>
-      </c>
-      <c r="R2" t="n">
-        <v>16</v>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>QA: Testing the throughput with standard/less packet sizes/varied user load in ESP mode</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>PCS-27972</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>594870</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>PCS-28018</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>May21-Performance</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>balachandras</t>
-        </is>
-      </c>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" t="n">
-        <v>4</v>
-      </c>
-      <c r="M3" t="n">
-        <v>57600</v>
-      </c>
-      <c r="N3" t="n">
-        <v>16</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>57600</v>
-      </c>
-      <c r="R3" t="n">
-        <v>16</v>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">QA:SM HW : ESP Max Users/Tunnel Setup count </t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>PCS-27539</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>593251</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>PCS-28018</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>May21-Performance</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>balachandras</t>
-        </is>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>4</v>
-      </c>
-      <c r="M4" t="n">
-        <v>57600</v>
-      </c>
-      <c r="N4" t="n">
-        <v>16</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>57600</v>
-      </c>
-      <c r="R4" t="n">
-        <v>16</v>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>Planning to validate RAID and LVM testing</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>PCS-25735</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>583642</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>PCS-28018</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>May21-Performance</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>balachandras</t>
-        </is>
-      </c>
-      <c r="K5" t="n">
-        <v>75</v>
-      </c>
-      <c r="L5" t="n">
-        <v>4</v>
-      </c>
-      <c r="M5" t="n">
-        <v>57600</v>
-      </c>
-      <c r="N5" t="n">
-        <v>16</v>
-      </c>
-      <c r="O5" t="n">
-        <v>43200</v>
-      </c>
-      <c r="P5" t="n">
-        <v>12</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>57600</v>
-      </c>
-      <c r="R5" t="n">
-        <v>16</v>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>PCS-2112</t>
-        </is>
-      </c>
-      <c r="V5" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>QA: Testing the HW-RAID controller functionality</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>PCS-28004</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>594947</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>PCS-28042</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>44261</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H6" s="2" t="n">
-        <v>44261</v>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>May21-ISA8000x-Support</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>balajit</t>
-        </is>
-      </c>
-      <c r="K6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" t="n">
-        <v>4</v>
-      </c>
-      <c r="M6" t="n">
-        <v>57600</v>
-      </c>
-      <c r="N6" t="n">
-        <v>16</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>57600</v>
-      </c>
-      <c r="R6" t="n">
-        <v>16</v>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>SM HW - ISA8000F Platform Testing, Code Review</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>PCS-28003</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>594946</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>PCS-28042</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F7" s="2" t="n">
-        <v>44261</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H7" s="2" t="n">
-        <v>44261</v>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>May21-ISA8000x-Support</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>balajit</t>
-        </is>
-      </c>
-      <c r="K7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" t="n">
-        <v>4</v>
-      </c>
-      <c r="M7" t="n">
-        <v>57600</v>
-      </c>
-      <c r="N7" t="n">
-        <v>16</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P7" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>57600</v>
-      </c>
-      <c r="R7" t="n">
-        <v>16</v>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y7" t="inlineStr">
-        <is>
-          <t>SM HW - ISA8000F Platform addition - License and UI Changes</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>PCS-28002</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>594945</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>PCS-28042</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F8" s="2" t="n">
-        <v>44261</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H8" s="2" t="n">
-        <v>44261</v>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>May21-ISA8000x-Support</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>balajit</t>
-        </is>
-      </c>
-      <c r="K8" t="n">
-        <v>96</v>
-      </c>
-      <c r="L8" t="n">
-        <v>6</v>
-      </c>
-      <c r="M8" t="n">
-        <v>86400</v>
-      </c>
-      <c r="N8" t="n">
-        <v>24</v>
-      </c>
-      <c r="O8" t="n">
-        <v>82800</v>
-      </c>
-      <c r="P8" t="n">
-        <v>23</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>3600</v>
-      </c>
-      <c r="R8" t="n">
-        <v>1</v>
-      </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="V8" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W8" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y8" t="inlineStr">
-        <is>
-          <t>SM HW - ISA8000F Platform addition - Platform changes</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>PCS-27971</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>594869</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>PCS-28017</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F9" s="2" t="n">
-        <v>44261</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H9" s="2" t="n">
-        <v>44261</v>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>May21-Deployment-Phase2</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>kalaimani.k</t>
-        </is>
-      </c>
-      <c r="K9" t="n">
-        <v>100</v>
-      </c>
-      <c r="L9" t="n">
-        <v>4</v>
-      </c>
-      <c r="M9" t="n">
-        <v>57600</v>
-      </c>
-      <c r="N9" t="n">
-        <v>16</v>
-      </c>
-      <c r="O9" t="n">
-        <v>57600</v>
-      </c>
-      <c r="P9" t="n">
-        <v>16</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>0</v>
-      </c>
-      <c r="R9" t="n">
-        <v>0</v>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="V9" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W9" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">SM-HW : ISA8000 - Make Coreboot/init changes as platform specific  </t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>PCS-27007</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>590473</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>PCS-28017</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F10" s="2" t="n">
-        <v>44261</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H10" s="2" t="n">
-        <v>44261</v>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>May21-Deployment-Phase2</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>kalaimani.k</t>
-        </is>
-      </c>
-      <c r="K10" t="n">
-        <v>25</v>
-      </c>
-      <c r="L10" t="n">
-        <v>8</v>
-      </c>
-      <c r="M10" t="n">
-        <v>115200</v>
-      </c>
-      <c r="N10" t="n">
-        <v>32</v>
-      </c>
-      <c r="O10" t="n">
-        <v>28800</v>
-      </c>
-      <c r="P10" t="n">
-        <v>8</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>86400</v>
-      </c>
-      <c r="R10" t="n">
-        <v>24</v>
-      </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>PCS-2118</t>
-        </is>
-      </c>
-      <c r="T10" t="inlineStr">
-        <is>
-          <t>PCS-2120</t>
-        </is>
-      </c>
-      <c r="U10" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="V10" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W10" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">SM-HW: ISA8000 Upgrade and Rollover Confirmation with LVM </t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>PCS-27969</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>594853</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>PCS-28017</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F11" s="2" t="n">
-        <v>44261</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H11" s="2" t="n">
-        <v>44261</v>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>May21-Deployment-Phase2</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>kalaimani.k</t>
-        </is>
-      </c>
-      <c r="K11" t="n">
-        <v>0</v>
-      </c>
-      <c r="L11" t="n">
-        <v>4</v>
-      </c>
-      <c r="M11" t="n">
-        <v>57600</v>
-      </c>
-      <c r="N11" t="n">
-        <v>16</v>
-      </c>
-      <c r="O11" t="n">
-        <v>0</v>
-      </c>
-      <c r="P11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>57600</v>
-      </c>
-      <c r="R11" t="n">
-        <v>16</v>
-      </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="V11" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W11" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y11" t="inlineStr">
-        <is>
-          <t>LVM: Support and bug fixes</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>PCS-27566</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>593427</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>PCS-28018</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>May21-Performance</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>karthikr</t>
-        </is>
-      </c>
-      <c r="K12" t="n">
-        <v>0</v>
-      </c>
-      <c r="L12" t="n">
-        <v>4</v>
-      </c>
-      <c r="M12" t="n">
-        <v>28800</v>
-      </c>
-      <c r="N12" t="n">
-        <v>8</v>
-      </c>
-      <c r="O12" t="n">
-        <v>0</v>
-      </c>
-      <c r="P12" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>28800</v>
-      </c>
-      <c r="R12" t="n">
-        <v>8</v>
-      </c>
-      <c r="S12" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="V12" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W12" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">QA: SMHW: Tunnel setup rate test for 25k Users on SSL mode </t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>PCS-27538</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>593250</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>PCS-28018</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>May21-Performance</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>karthikr</t>
-        </is>
-      </c>
-      <c r="K13" t="n">
-        <v>0</v>
-      </c>
-      <c r="L13" t="n">
-        <v>4</v>
-      </c>
-      <c r="M13" t="n">
-        <v>57600</v>
-      </c>
-      <c r="N13" t="n">
-        <v>16</v>
-      </c>
-      <c r="O13" t="n">
-        <v>0</v>
-      </c>
-      <c r="P13" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>57600</v>
-      </c>
-      <c r="R13" t="n">
-        <v>16</v>
-      </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="V13" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W13" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y13" t="inlineStr">
-        <is>
-          <t>QA: SM HW : Perform throughput tests with IMIX traffic(SSL)</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>PCS-27978</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>594893</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>PCS-28018</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>May21-Performance</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>karthikr</t>
-        </is>
-      </c>
-      <c r="K14" t="n">
-        <v>0</v>
-      </c>
-      <c r="L14" t="n">
-        <v>4</v>
-      </c>
-      <c r="M14" t="n">
-        <v>57600</v>
-      </c>
-      <c r="N14" t="n">
-        <v>16</v>
-      </c>
-      <c r="O14" t="n">
-        <v>0</v>
-      </c>
-      <c r="P14" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>57600</v>
-      </c>
-      <c r="R14" t="n">
-        <v>16</v>
-      </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="V14" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W14" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y14" t="inlineStr">
-        <is>
-          <t>QA: SM HW : SSL Max Throughput (25k Users/Tunnels, 1350 bytes)</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>PCS-27975</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>594885</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>PCS-28018</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>20-05-2021</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>17-06-2021</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>May21-Performance</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>karthikr</t>
-        </is>
-      </c>
-      <c r="K15" t="n">
-        <v>50</v>
-      </c>
-      <c r="L15" t="n">
-        <v>2</v>
-      </c>
-      <c r="M15" t="n">
-        <v>28800</v>
-      </c>
-      <c r="N15" t="n">
-        <v>8</v>
-      </c>
-      <c r="O15" t="n">
-        <v>14400</v>
-      </c>
-      <c r="P15" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>14400</v>
-      </c>
-      <c r="R15" t="n">
-        <v>4</v>
-      </c>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>PCS-2122</t>
-        </is>
-      </c>
-      <c r="V15" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="W15" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="Y15" t="inlineStr">
-        <is>
-          <t>QA: Build image from Build plan</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2887,13 +1440,6 @@
 END</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>EFFORT
-CONSUMED
-(IN HRS)</t>
-        </is>
-      </c>
       <c r="K1" t="inlineStr">
         <is>
           <t>Time spent
@@ -2996,7 +1542,7 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
         <v>57600</v>
@@ -3018,7 +1564,7 @@
         </is>
       </c>
       <c r="P2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
@@ -3074,7 +1620,7 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
         <v>57600</v>
@@ -3096,7 +1642,7 @@
         </is>
       </c>
       <c r="P3" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
@@ -3152,7 +1698,7 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
         <v>57600</v>
@@ -3174,7 +1720,7 @@
         </is>
       </c>
       <c r="P4" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
@@ -3230,7 +1776,7 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="K5" t="n">
         <v>57600</v>
@@ -3239,7 +1785,7 @@
         <v>16</v>
       </c>
       <c r="M5" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -3252,7 +1798,7 @@
         </is>
       </c>
       <c r="P5" t="n">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
@@ -3306,7 +1852,7 @@
         <v>44261</v>
       </c>
       <c r="J6" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
         <v>57600</v>
@@ -3326,7 +1872,7 @@
         <v>44261</v>
       </c>
       <c r="P6" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
@@ -3380,7 +1926,7 @@
         <v>44261</v>
       </c>
       <c r="J7" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
         <v>57600</v>
@@ -3400,7 +1946,7 @@
         <v>44261</v>
       </c>
       <c r="P7" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
@@ -3454,7 +2000,7 @@
         <v>44261</v>
       </c>
       <c r="J8" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K8" t="n">
         <v>86400</v>
@@ -3474,7 +2020,7 @@
         <v>44261</v>
       </c>
       <c r="P8" t="n">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
@@ -3548,7 +2094,7 @@
         <v>44261</v>
       </c>
       <c r="P9" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
@@ -3602,7 +2148,7 @@
         <v>44261</v>
       </c>
       <c r="J10" t="n">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="K10" t="n">
         <v>115200</v>
@@ -3622,7 +2168,7 @@
         <v>44261</v>
       </c>
       <c r="P10" t="n">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
@@ -3676,7 +2222,7 @@
         <v>44261</v>
       </c>
       <c r="J11" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
         <v>57600</v>
@@ -3696,7 +2242,7 @@
         <v>44261</v>
       </c>
       <c r="P11" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
@@ -3752,7 +2298,7 @@
         </is>
       </c>
       <c r="J12" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
         <v>28800</v>
@@ -3774,7 +2320,7 @@
         </is>
       </c>
       <c r="P12" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
@@ -3830,7 +2376,7 @@
         </is>
       </c>
       <c r="J13" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="K13" t="n">
         <v>57600</v>
@@ -3852,7 +2398,7 @@
         </is>
       </c>
       <c r="P13" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
@@ -3908,7 +2454,7 @@
         </is>
       </c>
       <c r="J14" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="K14" t="n">
         <v>57600</v>
@@ -3930,7 +2476,7 @@
         </is>
       </c>
       <c r="P14" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
@@ -3986,7 +2532,7 @@
         </is>
       </c>
       <c r="J15" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K15" t="n">
         <v>28800</v>
@@ -4008,7 +2554,7 @@
         </is>
       </c>
       <c r="P15" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="Q15" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
generated excel file from csv files as inputs
</commit_message>
<xml_diff>
--- a/excel_parser/generate-files.xlsx
+++ b/excel_parser/generate-files.xlsx
@@ -1440,6 +1440,13 @@
 END</t>
         </is>
       </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>ESTIMATED
+EFFORT
+(IN HRS))</t>
+        </is>
+      </c>
       <c r="K1" t="inlineStr">
         <is>
           <t>Time spent
@@ -1542,16 +1549,16 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K2" t="n">
-        <v>57600</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
         <v>16</v>
       </c>
       <c r="M2" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -1620,16 +1627,16 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K3" t="n">
-        <v>57600</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
         <v>16</v>
       </c>
       <c r="M3" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -1698,16 +1705,16 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K4" t="n">
-        <v>57600</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
         <v>16</v>
       </c>
       <c r="M4" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -1776,16 +1783,16 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="K5" t="n">
-        <v>57600</v>
+        <v>43200</v>
       </c>
       <c r="L5" t="n">
         <v>16</v>
       </c>
       <c r="M5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -1798,7 +1805,7 @@
         </is>
       </c>
       <c r="P5" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
@@ -1852,16 +1859,16 @@
         <v>44261</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K6" t="n">
-        <v>57600</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
         <v>16</v>
       </c>
       <c r="M6" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -1926,16 +1933,16 @@
         <v>44261</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K7" t="n">
-        <v>57600</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
         <v>16</v>
       </c>
       <c r="M7" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -2000,16 +2007,16 @@
         <v>44261</v>
       </c>
       <c r="J8" t="n">
+        <v>24</v>
+      </c>
+      <c r="K8" t="n">
+        <v>82800</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" t="n">
         <v>23</v>
-      </c>
-      <c r="K8" t="n">
-        <v>86400</v>
-      </c>
-      <c r="L8" t="n">
-        <v>24</v>
-      </c>
-      <c r="M8" t="n">
-        <v>1</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -2020,7 +2027,7 @@
         <v>44261</v>
       </c>
       <c r="P8" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
@@ -2080,10 +2087,10 @@
         <v>57600</v>
       </c>
       <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
         <v>16</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -2118,7 +2125,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>PCS-2118</t>
+          <t>PCS-2122</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -2148,16 +2155,16 @@
         <v>44261</v>
       </c>
       <c r="J10" t="n">
+        <v>32</v>
+      </c>
+      <c r="K10" t="n">
+        <v>28800</v>
+      </c>
+      <c r="L10" t="n">
+        <v>24</v>
+      </c>
+      <c r="M10" t="n">
         <v>8</v>
-      </c>
-      <c r="K10" t="n">
-        <v>115200</v>
-      </c>
-      <c r="L10" t="n">
-        <v>32</v>
-      </c>
-      <c r="M10" t="n">
-        <v>24</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -2168,7 +2175,7 @@
         <v>44261</v>
       </c>
       <c r="P10" t="n">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
@@ -2222,16 +2229,16 @@
         <v>44261</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K11" t="n">
-        <v>57600</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
         <v>16</v>
       </c>
       <c r="M11" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -2298,16 +2305,16 @@
         </is>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K12" t="n">
-        <v>28800</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
         <v>8</v>
       </c>
       <c r="M12" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
@@ -2376,16 +2383,16 @@
         </is>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K13" t="n">
-        <v>57600</v>
+        <v>0</v>
       </c>
       <c r="L13" t="n">
         <v>16</v>
       </c>
       <c r="M13" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="N13" t="inlineStr">
         <is>
@@ -2454,16 +2461,16 @@
         </is>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K14" t="n">
-        <v>57600</v>
+        <v>0</v>
       </c>
       <c r="L14" t="n">
         <v>16</v>
       </c>
       <c r="M14" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="N14" t="inlineStr">
         <is>
@@ -2532,13 +2539,13 @@
         </is>
       </c>
       <c r="J15" t="n">
+        <v>8</v>
+      </c>
+      <c r="K15" t="n">
+        <v>14400</v>
+      </c>
+      <c r="L15" t="n">
         <v>4</v>
-      </c>
-      <c r="K15" t="n">
-        <v>28800</v>
-      </c>
-      <c r="L15" t="n">
-        <v>8</v>
       </c>
       <c r="M15" t="n">
         <v>4</v>
@@ -2554,7 +2561,7 @@
         </is>
       </c>
       <c r="P15" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="Q15" t="inlineStr">
         <is>

</xml_diff>